<commit_message>
added doctor status to hide if not active
</commit_message>
<xml_diff>
--- a/records/report.xlsx
+++ b/records/report.xlsx
@@ -4497,8 +4497,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -4517,8 +4519,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -4537,8 +4541,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>

</xml_diff>